<commit_message>
Add name to all columns
</commit_message>
<xml_diff>
--- a/inst/extdata/questions.xlsx
+++ b/inst/extdata/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joses\Documents\_trabajo\packages\moodef\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA3F0FB-B4D8-46B1-8585-702818FD0CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF76AE1-2BF9-445D-8ADA-6629D4601302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>False</t>
   </si>
   <si>
-    <t>What basic operation does it have as a "+" symbol?</t>
-  </si>
-  <si>
     <t>Addition</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>a_3</t>
+  </si>
+  <si>
+    <t>What basic operation does it have as a + symbol?</t>
   </si>
 </sst>
 </file>
@@ -473,7 +473,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,13 +503,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -595,16 +595,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
@@ -621,19 +621,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -644,22 +644,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -670,54 +670,54 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>26</v>
-      </c>
-      <c r="H8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>25</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -725,19 +725,19 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -751,16 +751,16 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
@@ -777,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
vertical answers using v
</commit_message>
<xml_diff>
--- a/inst/extdata/questions.xlsx
+++ b/inst/extdata/questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joses\Documents\_trabajo\packages\moodef\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_seg\_trabajo\packages\moodef\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF76AE1-2BF9-445D-8ADA-6629D4601302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129843BF-C3FA-4F0E-903A-4AE750D4CD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
   <si>
     <t>type</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>What basic operation does it have as a + symbol?</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -472,9 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -696,7 +697,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>

</xml_diff>